<commit_message>
Update with Edited Lat/Lon
</commit_message>
<xml_diff>
--- a/Optimization Data.xlsx
+++ b/Optimization Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b424aae3153baf9/15.C57/Term Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53673889-3123-47D2-9593-D5F9917949EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{53673889-3123-47D2-9593-D5F9917949EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42B5A936-AA20-4635-B7ED-DCCC83CAA353}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4C982CF0-B96C-4C11-8705-E895C98B5AC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="94">
   <si>
     <t>G4800250950100</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>U7H001</t>
+  </si>
+  <si>
+    <t>EditLAT</t>
+  </si>
+  <si>
+    <t>EditLong</t>
   </si>
 </sst>
 </file>
@@ -683,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0E8E9D-880A-4AA3-B592-BC362DDBDCDD}">
-  <dimension ref="A1:BH10"/>
+  <dimension ref="A1:BJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="BC19" sqref="BC19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,9 +703,13 @@
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="10" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -880,8 +890,14 @@
       <c r="BH1" t="s">
         <v>91</v>
       </c>
+      <c r="BI1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -960,8 +976,14 @@
       <c r="BH2">
         <v>1712</v>
       </c>
+      <c r="BI2">
+        <v>28.596306999999999</v>
+      </c>
+      <c r="BJ2">
+        <v>-97.89425</v>
+      </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1040,8 +1062,14 @@
       <c r="BH3">
         <v>8083</v>
       </c>
+      <c r="BI3">
+        <v>28.325261999999999</v>
+      </c>
+      <c r="BJ3">
+        <v>-97.570344000000006</v>
+      </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1120,8 +1148,14 @@
       <c r="BH4">
         <v>2088</v>
       </c>
+      <c r="BI4">
+        <v>28.384394</v>
+      </c>
+      <c r="BJ4">
+        <v>-97.848106999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1200,8 +1234,14 @@
       <c r="BH5">
         <v>2910</v>
       </c>
+      <c r="BI5">
+        <v>28.460977</v>
+      </c>
+      <c r="BJ5">
+        <v>-97.661371000000003</v>
+      </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1280,8 +1320,14 @@
       <c r="BH6">
         <v>5135</v>
       </c>
+      <c r="BI6">
+        <v>28.420452999999998</v>
+      </c>
+      <c r="BJ6">
+        <v>-97.755132000000003</v>
+      </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1360,8 +1406,14 @@
       <c r="BH7">
         <v>1907</v>
       </c>
+      <c r="BI7">
+        <v>28.403562000000001</v>
+      </c>
+      <c r="BJ7">
+        <v>-97.759055000000004</v>
+      </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1440,8 +1492,14 @@
       <c r="BH8">
         <v>3394</v>
       </c>
+      <c r="BI8">
+        <v>28.397148000000001</v>
+      </c>
+      <c r="BJ8">
+        <v>-97.734679</v>
+      </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1520,8 +1578,14 @@
       <c r="BH9">
         <v>3545</v>
       </c>
+      <c r="BI9">
+        <v>28.388449999999999</v>
+      </c>
+      <c r="BJ9">
+        <v>-97.743106999999995</v>
+      </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1599,14 +1663,30 @@
       </c>
       <c r="BH10">
         <v>2273</v>
+      </c>
+      <c r="BI10">
+        <v>28.219092</v>
+      </c>
+      <c r="BJ10">
+        <v>-97.679786000000007</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D15C5FB97F1F4848BC2BB8B6F372C45A" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="112d604f9f2637135c0da1448cbb10db">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e2699ec7-7fec-4fa0-afbb-20ff63bd1169" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="56b384ee613323ecaa1a4c9c91c60fe1" ns3:_="">
     <xsd:import namespace="e2699ec7-7fec-4fa0-afbb-20ff63bd1169"/>
@@ -1756,15 +1836,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1774,6 +1845,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC29559D-805B-4688-9233-E6B9CEC68744}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBAD22C7-C4AE-42FF-9B23-3271C53E88C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1787,14 +1866,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC29559D-805B-4688-9233-E6B9CEC68744}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>